<commit_message>
Fix api manager app bug
</commit_message>
<xml_diff>
--- a/performance_test/a2_manuel.xlsx
+++ b/performance_test/a2_manuel.xlsx
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -95,7 +95,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +157,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -260,7 +259,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -352,11 +350,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="232761016"/>
-        <c:axId val="232759056"/>
+        <c:axId val="601658440"/>
+        <c:axId val="601659224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="232761016"/>
+        <c:axId val="601658440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,7 +391,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -460,7 +457,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232759056"/>
+        <c:crossAx val="601659224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -468,7 +465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="232759056"/>
+        <c:axId val="601659224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -514,7 +511,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -575,7 +571,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232761016"/>
+        <c:crossAx val="601658440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -668,7 +664,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -771,7 +766,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -919,7 +913,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1011,11 +1004,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92802712"/>
-        <c:axId val="92798400"/>
+        <c:axId val="603348528"/>
+        <c:axId val="603348136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92802712"/>
+        <c:axId val="603348528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,7 +1040,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1114,7 +1106,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92798400"/>
+        <c:crossAx val="603348136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1122,7 +1114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92798400"/>
+        <c:axId val="603348136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1168,7 +1160,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1229,7 +1220,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92802712"/>
+        <c:crossAx val="603348528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1322,7 +1313,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1424,9 +1414,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1466,7 +1454,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1510,9 +1497,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1552,7 +1537,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1595,7 +1579,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1642,7 +1625,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1650,7 +1632,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1680,7 +1661,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1725,7 +1705,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1817,11 +1796,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="230284056"/>
-        <c:axId val="230290720"/>
+        <c:axId val="603345392"/>
+        <c:axId val="603347744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="230284056"/>
+        <c:axId val="603345392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1858,7 +1837,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1925,7 +1903,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230290720"/>
+        <c:crossAx val="603347744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1933,7 +1911,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="230290720"/>
+        <c:axId val="603347744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,7 +1957,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2040,7 +2017,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230284056"/>
+        <c:crossAx val="603345392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2135,7 +2112,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2201,7 +2177,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2231,7 +2206,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2239,7 +2213,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2269,7 +2242,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2277,7 +2249,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -2307,7 +2278,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2350,7 +2320,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2393,7 +2362,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2436,7 +2404,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2479,7 +2446,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2524,7 +2490,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2616,11 +2581,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="230286800"/>
-        <c:axId val="230287976"/>
+        <c:axId val="603346960"/>
+        <c:axId val="603345784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="230286800"/>
+        <c:axId val="603346960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2652,7 +2617,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2719,7 +2683,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230287976"/>
+        <c:crossAx val="603345784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2727,7 +2691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="230287976"/>
+        <c:axId val="603345784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,7 +2737,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2834,7 +2797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="230286800"/>
+        <c:crossAx val="603346960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2927,7 +2890,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3028,7 +2990,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3071,7 +3032,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3114,7 +3074,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3157,7 +3116,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3200,7 +3158,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3243,7 +3200,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3286,7 +3242,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3331,7 +3286,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3423,11 +3377,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="691118968"/>
-        <c:axId val="691121320"/>
+        <c:axId val="603570256"/>
+        <c:axId val="603571040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="691118968"/>
+        <c:axId val="603570256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3464,7 +3418,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3531,7 +3484,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="691121320"/>
+        <c:crossAx val="603571040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3539,7 +3492,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="691121320"/>
+        <c:axId val="603571040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3585,7 +3538,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3646,7 +3598,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="691118968"/>
+        <c:crossAx val="603570256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3741,7 +3693,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3842,7 +3793,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3885,7 +3835,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3928,7 +3877,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3971,7 +3919,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4014,7 +3961,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4057,7 +4003,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4100,7 +4045,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -4145,7 +4089,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4237,11 +4180,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="691125632"/>
-        <c:axId val="691120928"/>
+        <c:axId val="603571432"/>
+        <c:axId val="603572608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="691125632"/>
+        <c:axId val="603571432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4273,7 +4216,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4340,7 +4282,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="691120928"/>
+        <c:crossAx val="603572608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4348,7 +4290,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="691120928"/>
+        <c:axId val="603572608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4394,7 +4336,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4455,7 +4396,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="691125632"/>
+        <c:crossAx val="603571432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4760,11 +4701,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="225038168"/>
-        <c:axId val="225035424"/>
+        <c:axId val="603572216"/>
+        <c:axId val="603573000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="225038168"/>
+        <c:axId val="603572216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4868,7 +4809,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225035424"/>
+        <c:crossAx val="603573000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4876,7 +4817,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="225035424"/>
+        <c:axId val="603573000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4983,7 +4924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225038168"/>
+        <c:crossAx val="603572216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5251,21 +5192,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$5</c:f>
+              <c:f>Sheet2!$H$2:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>63.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>71.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>63.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5350,11 +5291,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="693651504"/>
-        <c:axId val="693647192"/>
+        <c:axId val="603346568"/>
+        <c:axId val="603107768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="693651504"/>
+        <c:axId val="603346568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5458,7 +5399,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="693647192"/>
+        <c:crossAx val="603107768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5466,7 +5407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="693647192"/>
+        <c:axId val="603107768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5573,7 +5514,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="693651504"/>
+        <c:crossAx val="603346568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10896,10 +10837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10907,12 +10848,12 @@
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10931,8 +10872,11 @@
       <c r="F2">
         <v>8</v>
       </c>
+      <c r="H2">
+        <v>63.6</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10951,8 +10895,11 @@
       <c r="F3">
         <v>4</v>
       </c>
+      <c r="H3">
+        <v>70.400000000000006</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -10971,8 +10918,11 @@
       <c r="F4">
         <v>2</v>
       </c>
+      <c r="H4">
+        <v>71.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
@@ -10991,8 +10941,11 @@
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="H5">
+        <v>74</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>

</xml_diff>